<commit_message>
pilot version of task
</commit_message>
<xml_diff>
--- a/instructions/Instructions.xlsx
+++ b/instructions/Instructions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmuncy/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmuncy/Projects/cal_abstract/instructions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18237F42-B248-8642-B737-AD891FF8360D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED7C2A9-EA24-8046-8AFF-A0746515247C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48240" yWindow="4600" windowWidth="27640" windowHeight="16940" xr2:uid="{563E9E51-8460-9D46-9AAB-0239A769D758}"/>
+    <workbookView xWindow="46600" yWindow="4600" windowWidth="27640" windowHeight="16940" xr2:uid="{563E9E51-8460-9D46-9AAB-0239A769D758}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,16 +36,16 @@
     <t>For some images you should always press “Left”, and for others you should always press “Right” arrow key.</t>
   </si>
   <si>
-    <t>Some images are special, the correct response will the opposite of the preceding response. So, if you previously correctly responded “Left”, then the correct response would now be “Right”.</t>
-  </si>
-  <si>
     <t>After each response, you will be told whether you got the item correct or incorrect.</t>
   </si>
   <si>
-    <t>You can take as long as you like on each image, but the task will not continue until you press “Left” or “Right” arrow key.</t>
-  </si>
-  <si>
-    <t>This experiment will have three blocks, each block will take approximately 10 minutes to complete.</t>
+    <t>Some images are special: the correct response is the opposite of the preceding correct response. That is, if the previous correct answer was “Left” then the correct response would now be “Right”.</t>
+  </si>
+  <si>
+    <t>You can take as long as you like on each image, but the task will not continue until you press the “Left” or “Right” arrow key.</t>
+  </si>
+  <si>
+    <t>The experiment will have three blocks, each block will take approximately 10 minutes to complete.</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD1243F8-8AC2-F349-A031-0AB8FD5AED57}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -425,12 +425,12 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
@@ -443,8 +443,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updates for image dim, subj blocks, instructions
</commit_message>
<xml_diff>
--- a/instructions/Instructions.xlsx
+++ b/instructions/Instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmuncy/Projects/cal_abstract/instructions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED7C2A9-EA24-8046-8AFF-A0746515247C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F4A761-7338-E841-ACBF-9B107BFD4687}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="46600" yWindow="4600" windowWidth="27640" windowHeight="16940" xr2:uid="{563E9E51-8460-9D46-9AAB-0239A769D758}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Text</t>
   </si>
@@ -39,13 +39,16 @@
     <t>After each response, you will be told whether you got the item correct or incorrect.</t>
   </si>
   <si>
-    <t>Some images are special: the correct response is the opposite of the preceding correct response. That is, if the previous correct answer was “Left” then the correct response would now be “Right”.</t>
-  </si>
-  <si>
     <t>You can take as long as you like on each image, but the task will not continue until you press the “Left” or “Right” arrow key.</t>
   </si>
   <si>
     <t>The experiment will have three blocks, each block will take approximately 10 minutes to complete.</t>
+  </si>
+  <si>
+    <t>Some images are special: the correct response is the opposite of the preceding correct response.</t>
+  </si>
+  <si>
+    <t>That is, if the previous correct answer was “Left” then the correct response would now be “Right”.</t>
   </si>
 </sst>
 </file>
@@ -400,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD1243F8-8AC2-F349-A031-0AB8FD5AED57}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -425,22 +428,27 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
@@ -448,6 +456,9 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>